<commit_message>
Backup Baker Andina only lacking filters for 'País' and 'Departamento'
</commit_message>
<xml_diff>
--- a/Tabela_Transformada_BA.xlsx
+++ b/Tabela_Transformada_BA.xlsx
@@ -587,7 +587,7 @@
       <c r="I2" s="4" t="inlineStr"/>
       <c r="J2" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="K2" s="2" t="inlineStr"/>
@@ -623,7 +623,7 @@
       <c r="L3" s="4" t="inlineStr"/>
       <c r="M3" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="N3" s="2" t="inlineStr"/>
@@ -652,7 +652,7 @@
       <c r="H4" s="4" t="inlineStr"/>
       <c r="I4" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="J4" s="2" t="inlineStr"/>
@@ -688,7 +688,7 @@
       <c r="K5" s="4" t="inlineStr"/>
       <c r="L5" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="M5" s="2" t="inlineStr"/>
@@ -715,7 +715,7 @@
       <c r="E6" s="4" t="inlineStr"/>
       <c r="F6" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="G6" s="2" t="inlineStr"/>
@@ -751,7 +751,7 @@
       <c r="L7" s="4" t="inlineStr"/>
       <c r="M7" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="N7" s="2" t="inlineStr"/>
@@ -777,7 +777,7 @@
       <c r="I8" s="4" t="inlineStr"/>
       <c r="J8" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="K8" s="2" t="inlineStr"/>
@@ -807,7 +807,7 @@
       <c r="F9" s="4" t="inlineStr"/>
       <c r="G9" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr"/>
@@ -839,7 +839,7 @@
       <c r="E10" s="4" t="inlineStr"/>
       <c r="F10" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="G10" s="2" t="inlineStr"/>
@@ -873,7 +873,7 @@
       <c r="F11" s="4" t="inlineStr"/>
       <c r="G11" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="H11" s="2" t="inlineStr"/>
@@ -910,7 +910,7 @@
       <c r="J12" s="4" t="inlineStr"/>
       <c r="K12" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="L12" s="2" t="inlineStr"/>
@@ -942,7 +942,7 @@
       <c r="I13" s="4" t="inlineStr"/>
       <c r="J13" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="K13" s="2" t="inlineStr"/>
@@ -971,7 +971,7 @@
       <c r="E14" s="4" t="inlineStr"/>
       <c r="F14" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="G14" s="2" t="inlineStr"/>
@@ -1007,7 +1007,7 @@
       <c r="H15" s="4" t="inlineStr"/>
       <c r="I15" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="J15" s="2" t="inlineStr"/>
@@ -1035,7 +1035,7 @@
       <c r="G16" s="4" t="inlineStr"/>
       <c r="H16" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="I16" s="2" t="inlineStr"/>
@@ -1070,7 +1070,7 @@
       <c r="I17" s="4" t="inlineStr"/>
       <c r="J17" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="K17" s="2" t="inlineStr"/>
@@ -1101,7 +1101,7 @@
       <c r="G18" s="4" t="inlineStr"/>
       <c r="H18" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="I18" s="2" t="inlineStr"/>
@@ -1130,7 +1130,7 @@
       <c r="G19" s="4" t="inlineStr"/>
       <c r="H19" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="I19" s="2" t="inlineStr"/>
@@ -1164,7 +1164,7 @@
       <c r="H20" s="4" t="inlineStr"/>
       <c r="I20" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="J20" s="2" t="inlineStr"/>
@@ -1196,7 +1196,7 @@
       <c r="G21" s="4" t="inlineStr"/>
       <c r="H21" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="I21" s="2" t="inlineStr"/>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="N22" s="3" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="O22" s="2" t="inlineStr"/>
@@ -1256,7 +1256,7 @@
       <c r="E23" s="4" t="inlineStr"/>
       <c r="F23" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="G23" s="2" t="inlineStr"/>
@@ -1287,7 +1287,7 @@
       <c r="G24" s="4" t="inlineStr"/>
       <c r="H24" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="I24" s="2" t="inlineStr"/>
@@ -1322,7 +1322,7 @@
       <c r="M25" s="4" t="inlineStr"/>
       <c r="N25" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="O25" s="2" t="inlineStr"/>
@@ -1349,7 +1349,7 @@
       <c r="G26" s="4" t="inlineStr"/>
       <c r="H26" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="I26" s="2" t="inlineStr"/>
@@ -1388,7 +1388,7 @@
       <c r="M27" s="4" t="inlineStr"/>
       <c r="N27" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="O27" s="2" t="inlineStr"/>
@@ -1417,7 +1417,7 @@
       <c r="I28" s="4" t="inlineStr"/>
       <c r="J28" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="K28" s="2" t="inlineStr"/>
@@ -1448,7 +1448,7 @@
       <c r="G29" s="4" t="inlineStr"/>
       <c r="H29" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="I29" s="2" t="inlineStr"/>
@@ -1482,7 +1482,7 @@
       <c r="H30" s="4" t="inlineStr"/>
       <c r="I30" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="J30" s="2" t="inlineStr"/>
@@ -1519,7 +1519,7 @@
       <c r="L31" s="4" t="inlineStr"/>
       <c r="M31" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="N31" s="2" t="inlineStr"/>
@@ -1549,7 +1549,7 @@
       <c r="M32" s="4" t="inlineStr"/>
       <c r="N32" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="O32" s="2" t="inlineStr"/>
@@ -1574,7 +1574,7 @@
       <c r="E33" s="4" t="inlineStr"/>
       <c r="F33" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="G33" s="2" t="inlineStr"/>
@@ -1614,7 +1614,7 @@
       <c r="L34" s="4" t="inlineStr"/>
       <c r="M34" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="N34" s="2" t="inlineStr"/>
@@ -1641,7 +1641,7 @@
       <c r="F35" s="4" t="inlineStr"/>
       <c r="G35" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="H35" s="2" t="inlineStr"/>
@@ -1671,7 +1671,7 @@
       <c r="G36" s="4" t="inlineStr"/>
       <c r="H36" s="5" t="inlineStr">
         <is>
-          <t>06/2024</t>
+          <t>06/2026</t>
         </is>
       </c>
       <c r="I36" s="2" t="inlineStr"/>
@@ -1700,7 +1700,7 @@
       <c r="G37" s="4" t="inlineStr"/>
       <c r="H37" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="I37" s="2" t="inlineStr"/>
@@ -1735,7 +1735,7 @@
       <c r="M38" s="4" t="inlineStr"/>
       <c r="N38" s="5" t="inlineStr">
         <is>
-          <t>06/2024</t>
+          <t>06/2026</t>
         </is>
       </c>
       <c r="O38" s="2" t="inlineStr"/>
@@ -1764,7 +1764,7 @@
       <c r="M39" s="4" t="inlineStr"/>
       <c r="N39" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="O39" s="2" t="inlineStr"/>
@@ -1796,7 +1796,7 @@
       <c r="L40" s="4" t="inlineStr"/>
       <c r="M40" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="N40" s="2" t="inlineStr"/>
@@ -1828,7 +1828,7 @@
       <c r="K41" s="4" t="inlineStr"/>
       <c r="L41" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="M41" s="2" t="inlineStr"/>
@@ -1859,7 +1859,7 @@
       <c r="I42" s="4" t="inlineStr"/>
       <c r="J42" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="K42" s="2" t="inlineStr"/>
@@ -1894,7 +1894,7 @@
       <c r="K43" s="4" t="inlineStr"/>
       <c r="L43" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="M43" s="2" t="inlineStr"/>
@@ -1925,7 +1925,7 @@
       <c r="M44" s="4" t="inlineStr"/>
       <c r="N44" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="O44" s="2" t="inlineStr"/>
@@ -1959,7 +1959,7 @@
       <c r="N45" s="4" t="inlineStr"/>
       <c r="O45" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
     </row>
@@ -1988,7 +1988,7 @@
       <c r="J46" s="4" t="inlineStr"/>
       <c r="K46" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="L46" s="2" t="inlineStr"/>
@@ -2020,7 +2020,7 @@
       <c r="I47" s="4" t="inlineStr"/>
       <c r="J47" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="K47" s="2" t="inlineStr"/>
@@ -2054,7 +2054,7 @@
       <c r="J48" s="4" t="inlineStr"/>
       <c r="K48" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="L48" s="2" t="inlineStr"/>
@@ -2090,7 +2090,7 @@
       <c r="M49" s="4" t="inlineStr"/>
       <c r="N49" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="O49" s="2" t="inlineStr"/>
@@ -2121,7 +2121,7 @@
       <c r="K50" s="4" t="inlineStr"/>
       <c r="L50" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="M50" s="2" t="inlineStr"/>
@@ -2155,7 +2155,7 @@
       <c r="L51" s="4" t="inlineStr"/>
       <c r="M51" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="N51" s="2" t="inlineStr"/>
@@ -2185,7 +2185,7 @@
       <c r="M52" s="4" t="inlineStr"/>
       <c r="N52" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="O52" s="2" t="inlineStr"/>
@@ -2212,7 +2212,7 @@
       <c r="G53" s="4" t="inlineStr"/>
       <c r="H53" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="I53" s="2" t="inlineStr"/>
@@ -2271,7 +2271,7 @@
       <c r="H55" s="4" t="inlineStr"/>
       <c r="I55" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="J55" s="2" t="inlineStr"/>
@@ -2310,7 +2310,7 @@
       </c>
       <c r="O56" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
     </row>
@@ -2338,7 +2338,7 @@
       <c r="M57" s="4" t="inlineStr"/>
       <c r="N57" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="O57" s="2" t="inlineStr"/>
@@ -2361,7 +2361,7 @@
       <c r="G58" s="4" t="inlineStr"/>
       <c r="H58" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="I58" s="2" t="inlineStr"/>
@@ -2398,7 +2398,7 @@
       <c r="K59" s="4" t="inlineStr"/>
       <c r="L59" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="M59" s="2" t="inlineStr"/>
@@ -2431,7 +2431,7 @@
       <c r="K60" s="4" t="inlineStr"/>
       <c r="L60" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="M60" s="2" t="inlineStr"/>
@@ -2458,7 +2458,7 @@
       <c r="E61" s="4" t="inlineStr"/>
       <c r="F61" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="G61" s="2" t="inlineStr"/>
@@ -2493,7 +2493,7 @@
       <c r="G62" s="4" t="inlineStr"/>
       <c r="H62" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="I62" s="2" t="inlineStr"/>
@@ -2526,7 +2526,7 @@
       <c r="G63" s="4" t="inlineStr"/>
       <c r="H63" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="I63" s="2" t="inlineStr"/>
@@ -2561,7 +2561,7 @@
       <c r="I64" s="4" t="inlineStr"/>
       <c r="J64" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="K64" s="2" t="inlineStr"/>
@@ -2592,7 +2592,7 @@
       <c r="K65" s="4" t="inlineStr"/>
       <c r="L65" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="M65" s="2" t="inlineStr"/>
@@ -2625,7 +2625,7 @@
       <c r="K66" s="4" t="inlineStr"/>
       <c r="L66" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="M66" s="2" t="inlineStr"/>
@@ -2654,7 +2654,7 @@
       <c r="G67" s="4" t="inlineStr"/>
       <c r="H67" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="I67" s="2" t="inlineStr"/>
@@ -2693,7 +2693,7 @@
       <c r="M68" s="4" t="inlineStr"/>
       <c r="N68" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="O68" s="2" t="inlineStr"/>
@@ -2720,7 +2720,7 @@
       <c r="G69" s="4" t="inlineStr"/>
       <c r="H69" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="I69" s="2" t="inlineStr"/>
@@ -2751,7 +2751,7 @@
       <c r="E70" s="4" t="inlineStr"/>
       <c r="F70" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="G70" s="2" t="inlineStr"/>
@@ -2790,7 +2790,7 @@
       <c r="K71" s="4" t="inlineStr"/>
       <c r="L71" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="M71" s="2" t="inlineStr"/>
@@ -2819,7 +2819,7 @@
       <c r="G72" s="4" t="inlineStr"/>
       <c r="H72" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="I72" s="2" t="inlineStr"/>
@@ -2859,7 +2859,7 @@
       <c r="N73" s="4" t="inlineStr"/>
       <c r="O73" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
     </row>
@@ -2886,7 +2886,7 @@
       <c r="H74" s="4" t="inlineStr"/>
       <c r="I74" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="J74" s="2" t="inlineStr"/>
@@ -2915,7 +2915,7 @@
       <c r="H75" s="4" t="inlineStr"/>
       <c r="I75" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="J75" s="2" t="inlineStr"/>
@@ -2947,7 +2947,7 @@
       <c r="G76" s="4" t="inlineStr"/>
       <c r="H76" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="I76" s="2" t="inlineStr"/>
@@ -2979,7 +2979,7 @@
       <c r="F77" s="4" t="inlineStr"/>
       <c r="G77" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="H77" s="2" t="inlineStr"/>
@@ -3020,7 +3020,7 @@
       </c>
       <c r="O78" s="5" t="inlineStr">
         <is>
-          <t>12/2023</t>
+          <t>12/2025</t>
         </is>
       </c>
     </row>
@@ -3050,7 +3050,7 @@
       <c r="K79" s="4" t="inlineStr"/>
       <c r="L79" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="M79" s="2" t="inlineStr"/>
@@ -3077,7 +3077,7 @@
       <c r="E80" s="4" t="inlineStr"/>
       <c r="F80" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="G80" s="2" t="inlineStr"/>
@@ -3116,7 +3116,7 @@
       <c r="K81" s="4" t="inlineStr"/>
       <c r="L81" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="M81" s="2" t="inlineStr"/>
@@ -3148,7 +3148,7 @@
       <c r="J82" s="4" t="inlineStr"/>
       <c r="K82" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="L82" s="2" t="inlineStr"/>
@@ -3176,7 +3176,7 @@
       <c r="I83" s="4" t="inlineStr"/>
       <c r="J83" s="5" t="inlineStr">
         <is>
-          <t>06/2024</t>
+          <t>06/2026</t>
         </is>
       </c>
       <c r="K83" s="2" t="inlineStr"/>
@@ -3214,7 +3214,7 @@
       </c>
       <c r="O84" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
     </row>
@@ -3237,7 +3237,7 @@
       <c r="H85" s="4" t="inlineStr"/>
       <c r="I85" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="J85" s="2" t="inlineStr"/>
@@ -3271,7 +3271,7 @@
       <c r="I86" s="4" t="inlineStr"/>
       <c r="J86" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="K86" s="2" t="inlineStr"/>
@@ -3305,7 +3305,7 @@
       <c r="J87" s="4" t="inlineStr"/>
       <c r="K87" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="L87" s="2" t="inlineStr"/>
@@ -3340,7 +3340,7 @@
       <c r="L88" s="4" t="inlineStr"/>
       <c r="M88" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="N88" s="2" t="inlineStr"/>
@@ -3372,7 +3372,7 @@
       <c r="K89" s="4" t="inlineStr"/>
       <c r="L89" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="M89" s="2" t="inlineStr"/>
@@ -3406,7 +3406,7 @@
       <c r="L90" s="4" t="inlineStr"/>
       <c r="M90" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="N90" s="2" t="inlineStr"/>
@@ -3439,7 +3439,7 @@
       <c r="L91" s="4" t="inlineStr"/>
       <c r="M91" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="N91" s="2" t="inlineStr"/>
@@ -3469,7 +3469,7 @@
       <c r="I92" s="4" t="inlineStr"/>
       <c r="J92" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="K92" s="2" t="inlineStr"/>
@@ -3498,7 +3498,7 @@
       <c r="E93" s="4" t="inlineStr"/>
       <c r="F93" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="G93" s="2" t="inlineStr"/>
@@ -3533,7 +3533,7 @@
       <c r="G94" s="4" t="inlineStr"/>
       <c r="H94" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="I94" s="2" t="inlineStr"/>
@@ -3566,7 +3566,7 @@
       <c r="G95" s="4" t="inlineStr"/>
       <c r="H95" s="5" t="inlineStr">
         <is>
-          <t>09/2023</t>
+          <t>09/2025</t>
         </is>
       </c>
       <c r="I95" s="2" t="inlineStr"/>
@@ -3603,7 +3603,7 @@
       <c r="K96" s="4" t="inlineStr"/>
       <c r="L96" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="M96" s="2" t="inlineStr"/>
@@ -3632,7 +3632,7 @@
       <c r="G97" s="4" t="inlineStr"/>
       <c r="H97" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="I97" s="2" t="inlineStr"/>
@@ -3664,7 +3664,7 @@
       <c r="F98" s="4" t="inlineStr"/>
       <c r="G98" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="H98" s="2" t="inlineStr"/>
@@ -3701,7 +3701,7 @@
       <c r="J99" s="4" t="inlineStr"/>
       <c r="K99" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="L99" s="2" t="inlineStr"/>
@@ -3735,7 +3735,7 @@
       <c r="K100" s="4" t="inlineStr"/>
       <c r="L100" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="M100" s="2" t="inlineStr"/>
@@ -3768,7 +3768,7 @@
       <c r="K101" s="4" t="inlineStr"/>
       <c r="L101" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="M101" s="2" t="inlineStr"/>
@@ -3798,7 +3798,7 @@
       <c r="H102" s="4" t="inlineStr"/>
       <c r="I102" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="J102" s="2" t="inlineStr"/>
@@ -3830,7 +3830,7 @@
       <c r="K103" s="4" t="inlineStr"/>
       <c r="L103" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="M103" s="2" t="inlineStr"/>
@@ -3861,7 +3861,7 @@
       </c>
       <c r="N104" s="3" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="O104" s="2" t="inlineStr"/>
@@ -3888,7 +3888,7 @@
       <c r="G105" s="4" t="inlineStr"/>
       <c r="H105" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="I105" s="2" t="inlineStr"/>
@@ -3923,7 +3923,7 @@
       <c r="M106" s="4" t="inlineStr"/>
       <c r="N106" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="O106" s="2" t="inlineStr"/>
@@ -3952,7 +3952,7 @@
       <c r="I107" s="4" t="inlineStr"/>
       <c r="J107" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="K107" s="2" t="inlineStr"/>
@@ -3985,7 +3985,7 @@
       <c r="I108" s="4" t="inlineStr"/>
       <c r="J108" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="K108" s="2" t="inlineStr"/>
@@ -4014,7 +4014,7 @@
       <c r="E109" s="4" t="inlineStr"/>
       <c r="F109" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="G109" s="2" t="inlineStr"/>
@@ -4051,7 +4051,7 @@
       <c r="M110" s="4" t="inlineStr"/>
       <c r="N110" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="O110" s="2" t="inlineStr"/>
@@ -4105,7 +4105,7 @@
       <c r="E112" s="4" t="inlineStr"/>
       <c r="F112" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
       <c r="G112" s="2" t="inlineStr"/>
@@ -4139,7 +4139,7 @@
       <c r="J113" s="4" t="inlineStr"/>
       <c r="K113" s="5" t="inlineStr">
         <is>
-          <t>05/2024</t>
+          <t>05/2026</t>
         </is>
       </c>
       <c r="L113" s="2" t="inlineStr"/>
@@ -4169,7 +4169,7 @@
       <c r="G114" s="4" t="inlineStr"/>
       <c r="H114" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
       <c r="I114" s="2" t="inlineStr"/>
@@ -4280,7 +4280,7 @@
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
     </row>
@@ -4302,7 +4302,7 @@
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>07/2024</t>
+          <t>07/2026</t>
         </is>
       </c>
     </row>
@@ -4338,7 +4338,7 @@
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>04/2026</t>
         </is>
       </c>
     </row>

</xml_diff>